<commit_message>
Worked on marketing plan
</commit_message>
<xml_diff>
--- a/connection_matrix.xlsx
+++ b/connection_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470E7798-868A-4D00-B412-57AFA35563FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DA234C-7287-4904-AEBC-4C554BBDED83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E3E2C5C-514C-46EA-AB74-751DD2BA6F70}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
   <si>
     <t>Platforms</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>not important enough</t>
+  </si>
+  <si>
+    <t>Presskit</t>
+  </si>
+  <si>
+    <t>small link</t>
+  </si>
+  <si>
+    <t>Twitch page</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E910C1E-0AAC-4671-ABB9-E7E37A8B9B04}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,7 +502,7 @@
     <col min="10" max="10" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,8 +527,14 @@
       <c r="H1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -541,8 +556,11 @@
       <c r="H2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -567,8 +585,11 @@
       <c r="H3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -581,8 +602,11 @@
       <c r="H4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -604,8 +628,11 @@
       <c r="H5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -630,8 +657,11 @@
       <c r="H6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -656,8 +686,11 @@
       <c r="H7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -683,12 +716,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>